<commit_message>
[ProjRech] Fin tête disc et trans, nettoyage
</commit_message>
<xml_diff>
--- a/master2/output/heads_disc_Fr_0.003_Oc_0.025_NbH_356_TotDD_606.xlsx
+++ b/master2/output/heads_disc_Fr_0.003_Oc_0.025_NbH_356_TotDD_606.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6257C0B9-0740-43CC-94B9-7C46E6E8B8B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A7A6ED-51D4-49F9-BAEF-89315A4A786F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21330" yWindow="2670" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplinary" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Damien Gouteux</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{973A6420-AE1D-4576-8C57-CC9803FD2728}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Damien Gouteux:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Les lemmes différents</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{09320CB7-841D-4601-9A95-EBA4D92C284F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Damien Gouteux:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Les occurrences de lemmes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2652" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2654" uniqueCount="771">
   <si>
     <t>Dom</t>
   </si>
@@ -2338,6 +2396,12 @@
   </si>
   <si>
     <t>sur sel</t>
+  </si>
+  <si>
+    <t>Kept A occ</t>
+  </si>
+  <si>
+    <t>% D / E</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2411,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2376,6 +2440,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2745,23 +2822,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="9" max="10" width="9.140625" style="5"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="11" max="12" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2772,28 +2851,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>766</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2804,30 +2889,37 @@
         <v>2579</v>
       </c>
       <c r="D2">
+        <v>250</v>
+      </c>
+      <c r="E2">
         <v>6942</v>
       </c>
-      <c r="E2" s="5">
-        <f>C2/D2</f>
+      <c r="F2" s="5">
+        <f>D2/E2</f>
+        <v>3.6012676462114666E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <f>C2/E2</f>
         <v>0.37150677038317487</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>36</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>1.3958898797983709E-2</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>7</v>
       </c>
-      <c r="I2" s="5">
-        <f>H2/F2</f>
+      <c r="K2" s="5">
+        <f>J2/H2</f>
         <v>0.19444444444444445</v>
       </c>
-      <c r="J2" s="16">
+      <c r="L2" s="16">
         <v>2.7142303218301669E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2838,30 +2930,37 @@
         <v>3444</v>
       </c>
       <c r="D3">
+        <v>2834</v>
+      </c>
+      <c r="E3">
         <v>13391</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E26" si="0">C3/D3</f>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F26" si="0">D3/E3</f>
+        <v>0.21163468000896124</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G26" si="1">C3/E3</f>
         <v>0.25718766335598536</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>43</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>1.2485481997677119E-2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>34</v>
       </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I3:I26" si="1">H3/F3</f>
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K26" si="2">J3/H3</f>
         <v>0.79069767441860461</v>
       </c>
-      <c r="J3" s="10">
+      <c r="L3" s="10">
         <v>9.8722415795586532E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2872,30 +2971,37 @@
         <v>1624</v>
       </c>
       <c r="D4">
+        <v>528</v>
+      </c>
+      <c r="E4">
         <v>4629</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <f t="shared" si="0"/>
+        <v>0.11406351263771873</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="1"/>
         <v>0.35083171311298339</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>53</v>
       </c>
-      <c r="G4" s="5">
+      <c r="I4" s="5">
         <v>3.2635467980295568E-2</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>15</v>
       </c>
-      <c r="I4" s="5">
-        <f t="shared" si="1"/>
+      <c r="K4" s="5">
+        <f t="shared" si="2"/>
         <v>0.28301886792452829</v>
       </c>
-      <c r="J4" s="10">
+      <c r="L4" s="10">
         <v>9.2364532019704442E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2906,30 +3012,37 @@
         <v>3376</v>
       </c>
       <c r="D5">
+        <v>963</v>
+      </c>
+      <c r="E5">
         <v>8685</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <f t="shared" si="0"/>
+        <v>0.11088082901554404</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="1"/>
         <v>0.38871617731721358</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>33</v>
       </c>
-      <c r="G5" s="5">
+      <c r="I5" s="5">
         <v>9.774881516587678E-3</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>19</v>
       </c>
-      <c r="I5" s="5">
-        <f t="shared" si="1"/>
+      <c r="K5" s="5">
+        <f t="shared" si="2"/>
         <v>0.5757575757575758</v>
       </c>
-      <c r="J5" s="10">
+      <c r="L5" s="10">
         <v>5.6279620853080569E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2940,30 +3053,37 @@
         <v>788</v>
       </c>
       <c r="D6">
+        <v>523</v>
+      </c>
+      <c r="E6">
         <v>2710</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
+        <v>0.19298892988929889</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="1"/>
         <v>0.29077490774907749</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>54</v>
       </c>
-      <c r="G6" s="8">
+      <c r="I6" s="8">
         <v>6.8527918781725886E-2</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>19</v>
       </c>
-      <c r="I6" s="5">
-        <f t="shared" si="1"/>
+      <c r="K6" s="5">
+        <f t="shared" si="2"/>
         <v>0.35185185185185186</v>
       </c>
-      <c r="J6" s="15">
+      <c r="L6" s="15">
         <v>2.4111675126903549E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2974,30 +3094,37 @@
         <v>4189</v>
       </c>
       <c r="D7">
+        <v>6084</v>
+      </c>
+      <c r="E7">
         <v>26398</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <f t="shared" si="0"/>
+        <v>0.23047200545495872</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
         <v>0.15868626411091749</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>45</v>
       </c>
-      <c r="G7" s="5">
+      <c r="I7" s="5">
         <v>1.0742420625447601E-2</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>38</v>
       </c>
-      <c r="I7" s="5">
-        <f t="shared" si="1"/>
+      <c r="K7" s="5">
+        <f t="shared" si="2"/>
         <v>0.84444444444444444</v>
       </c>
-      <c r="J7" s="10">
+      <c r="L7" s="10">
         <v>9.0713774170446404E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3007,31 +3134,38 @@
       <c r="C8">
         <v>273</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="14">
         <v>489</v>
       </c>
-      <c r="E8" s="8">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
+        <v>1.6359918200408999E-2</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="1"/>
         <v>0.55828220858895705</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>79</v>
       </c>
-      <c r="G8" s="8">
+      <c r="I8" s="8">
         <v>0.2893772893772894</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="I8" s="11">
-        <f t="shared" si="1"/>
+      <c r="K8" s="11">
+        <f t="shared" si="2"/>
         <v>5.0632911392405063E-2</v>
       </c>
-      <c r="J8" s="10">
+      <c r="L8" s="10">
         <v>1.465201465201465E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3042,30 +3176,37 @@
         <v>1786</v>
       </c>
       <c r="D9">
+        <v>2254</v>
+      </c>
+      <c r="E9">
         <v>9445</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
+        <v>0.23864478560084701</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
         <v>0.18909475913181578</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>67</v>
       </c>
-      <c r="G9" s="5">
+      <c r="I9" s="5">
         <v>3.7513997760358353E-2</v>
       </c>
-      <c r="H9">
-        <v>37</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <v>37</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="2"/>
         <v>0.55223880597014929</v>
       </c>
-      <c r="J9" s="15">
+      <c r="L9" s="15">
         <v>2.0716685330347141E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3075,31 +3216,38 @@
       <c r="C10">
         <v>604</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10" s="14">
         <v>1191</v>
       </c>
-      <c r="E10" s="8">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
+        <v>3.0226700251889168E-2</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
         <v>0.50713685978169609</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>63</v>
       </c>
-      <c r="G10" s="8">
+      <c r="I10" s="8">
         <v>0.1043046357615894</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="I10" s="11">
-        <f t="shared" si="1"/>
+      <c r="K10" s="11">
+        <f t="shared" si="2"/>
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="J10" s="10">
+      <c r="L10" s="10">
         <v>4.9668874172185433E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3110,30 +3258,37 @@
         <v>3546</v>
       </c>
       <c r="D11">
+        <v>9238</v>
+      </c>
+      <c r="E11">
         <v>25955</v>
       </c>
-      <c r="E11" s="5">
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
+        <v>0.35592371412059332</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
         <v>0.13662107493739165</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>51</v>
       </c>
-      <c r="G11" s="5">
+      <c r="I11" s="5">
         <v>1.4382402707275799E-2</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>50</v>
       </c>
-      <c r="I11" s="8">
-        <f t="shared" si="1"/>
+      <c r="K11" s="8">
+        <f t="shared" si="2"/>
         <v>0.98039215686274506</v>
       </c>
-      <c r="J11" s="10">
+      <c r="L11" s="10">
         <v>1.410039481105471E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3144,30 +3299,37 @@
         <v>7005</v>
       </c>
       <c r="D12">
+        <v>2367</v>
+      </c>
+      <c r="E12">
         <v>25671</v>
       </c>
-      <c r="E12" s="5">
+      <c r="F12" s="5">
         <f t="shared" si="0"/>
+        <v>9.2205212107046866E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
         <v>0.2728760079467103</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>23</v>
       </c>
-      <c r="G12" s="11">
+      <c r="I12" s="11">
         <v>3.2833690221270519E-3</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>19</v>
       </c>
-      <c r="I12" s="5">
-        <f t="shared" si="1"/>
+      <c r="K12" s="5">
+        <f t="shared" si="2"/>
         <v>0.82608695652173914</v>
       </c>
-      <c r="J12" s="16">
+      <c r="L12" s="16">
         <v>2.7123483226266952E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3178,30 +3340,37 @@
         <v>3281</v>
       </c>
       <c r="D13">
+        <v>6425</v>
+      </c>
+      <c r="E13">
         <v>16241</v>
       </c>
-      <c r="E13" s="5">
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
+        <v>0.39560371898282126</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
         <v>0.20201958007511853</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>58</v>
       </c>
-      <c r="G13" s="5">
+      <c r="I13" s="5">
         <v>1.7677537336177999E-2</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>49</v>
       </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
+      <c r="K13" s="5">
+        <f t="shared" si="2"/>
         <v>0.84482758620689657</v>
       </c>
-      <c r="J13" s="10">
+      <c r="L13" s="10">
         <v>1.4934471197805549E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3212,30 +3381,37 @@
         <v>3435</v>
       </c>
       <c r="D14">
+        <v>3120</v>
+      </c>
+      <c r="E14">
         <v>15512</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F14" s="5">
         <f t="shared" si="0"/>
+        <v>0.20113460546673542</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="1"/>
         <v>0.22144146467251161</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>52</v>
       </c>
-      <c r="G14" s="5">
+      <c r="I14" s="5">
         <v>1.513828238719068E-2</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>35</v>
       </c>
-      <c r="I14" s="5">
-        <f t="shared" si="1"/>
+      <c r="K14" s="5">
+        <f t="shared" si="2"/>
         <v>0.67307692307692313</v>
       </c>
-      <c r="J14" s="10">
+      <c r="L14" s="10">
         <v>1.018922852983988E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3246,30 +3422,37 @@
         <v>5142</v>
       </c>
       <c r="D15">
+        <v>1716</v>
+      </c>
+      <c r="E15">
         <v>14278</v>
       </c>
-      <c r="E15" s="5">
+      <c r="F15" s="5">
         <f t="shared" si="0"/>
+        <v>0.12018489984591679</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="1"/>
         <v>0.3601344726152122</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>34</v>
       </c>
-      <c r="G15" s="5">
+      <c r="I15" s="5">
         <v>6.6122131466355514E-3</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>25</v>
       </c>
-      <c r="I15" s="5">
-        <f t="shared" si="1"/>
+      <c r="K15" s="5">
+        <f t="shared" si="2"/>
         <v>0.73529411764705888</v>
       </c>
-      <c r="J15" s="10">
+      <c r="L15" s="10">
         <v>4.8619214313496686E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3280,30 +3463,37 @@
         <v>888</v>
       </c>
       <c r="D16">
+        <v>414</v>
+      </c>
+      <c r="E16">
         <v>2745</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
+        <v>0.15081967213114755</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
         <v>0.32349726775956283</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>64</v>
       </c>
-      <c r="G16" s="8">
+      <c r="I16" s="8">
         <v>7.2072072072072071E-2</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>21</v>
       </c>
-      <c r="I16" s="5">
-        <f t="shared" si="1"/>
+      <c r="K16" s="5">
+        <f t="shared" si="2"/>
         <v>0.328125</v>
       </c>
-      <c r="J16" s="15">
+      <c r="L16" s="15">
         <v>2.364864864864865E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3314,30 +3504,37 @@
         <v>2800</v>
       </c>
       <c r="D17">
+        <v>735</v>
+      </c>
+      <c r="E17">
         <v>7856</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <f t="shared" si="0"/>
+        <v>9.3559063136456205E-2</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="1"/>
         <v>0.35641547861507128</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>35</v>
       </c>
-      <c r="G17" s="5">
+      <c r="I17" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>16</v>
       </c>
-      <c r="I17" s="5">
-        <f t="shared" si="1"/>
+      <c r="K17" s="5">
+        <f t="shared" si="2"/>
         <v>0.45714285714285713</v>
       </c>
-      <c r="J17" s="10">
+      <c r="L17" s="10">
         <v>5.7142857142857143E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3348,30 +3545,37 @@
         <v>3603</v>
       </c>
       <c r="D18">
+        <v>14839</v>
+      </c>
+      <c r="E18">
         <v>30667</v>
       </c>
-      <c r="E18" s="11">
+      <c r="F18" s="5">
         <f t="shared" si="0"/>
+        <v>0.48387517526983403</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="1"/>
         <v>0.1174878533928979</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>49</v>
       </c>
-      <c r="G18" s="5">
+      <c r="I18" s="5">
         <v>1.3599777962808771E-2</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>47</v>
       </c>
-      <c r="I18" s="8">
-        <f t="shared" si="1"/>
+      <c r="K18" s="8">
+        <f t="shared" si="2"/>
         <v>0.95918367346938771</v>
       </c>
-      <c r="J18" s="10">
+      <c r="L18" s="10">
         <v>1.304468498473494E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3382,30 +3586,37 @@
         <v>1245</v>
       </c>
       <c r="D19">
+        <v>211</v>
+      </c>
+      <c r="E19">
         <v>3675</v>
       </c>
-      <c r="E19" s="5">
+      <c r="F19" s="5">
         <f t="shared" si="0"/>
+        <v>5.7414965986394555E-2</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
         <v>0.33877551020408164</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>53</v>
       </c>
-      <c r="G19" s="5">
+      <c r="I19" s="5">
         <v>4.257028112449799E-2</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>13</v>
       </c>
-      <c r="I19" s="5">
-        <f t="shared" si="1"/>
+      <c r="K19" s="5">
+        <f t="shared" si="2"/>
         <v>0.24528301886792453</v>
       </c>
-      <c r="J19" s="10">
+      <c r="L19" s="10">
         <v>1.044176706827309E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3416,30 +3627,37 @@
         <v>943</v>
       </c>
       <c r="D20">
+        <v>101</v>
+      </c>
+      <c r="E20">
         <v>2663</v>
       </c>
-      <c r="E20" s="5">
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
+        <v>3.7927149831017651E-2</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
         <v>0.35411190386781827</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>66</v>
       </c>
-      <c r="G20" s="8">
+      <c r="I20" s="8">
         <v>6.9989395546129374E-2</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>8</v>
       </c>
-      <c r="I20" s="5">
-        <f t="shared" si="1"/>
+      <c r="K20" s="5">
+        <f t="shared" si="2"/>
         <v>0.12121212121212122</v>
       </c>
-      <c r="J20" s="10">
+      <c r="L20" s="10">
         <v>8.483563096500531E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3450,30 +3668,37 @@
         <v>2520</v>
       </c>
       <c r="D21">
+        <v>1204</v>
+      </c>
+      <c r="E21">
         <v>9864</v>
       </c>
-      <c r="E21" s="5">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
+        <v>0.12206001622060016</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
         <v>0.25547445255474455</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>49</v>
       </c>
-      <c r="G21" s="5">
+      <c r="I21" s="5">
         <v>1.9444444444444441E-2</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>23</v>
       </c>
-      <c r="I21" s="5">
-        <f t="shared" si="1"/>
+      <c r="K21" s="5">
+        <f t="shared" si="2"/>
         <v>0.46938775510204084</v>
       </c>
-      <c r="J21" s="10">
+      <c r="L21" s="10">
         <v>9.1269841269841275E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3484,30 +3709,37 @@
         <v>1164</v>
       </c>
       <c r="D22">
+        <v>52</v>
+      </c>
+      <c r="E22">
         <v>3141</v>
       </c>
-      <c r="E22" s="5">
+      <c r="F22" s="5">
         <f t="shared" si="0"/>
+        <v>1.6555237185609677E-2</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="1"/>
         <v>0.37058261700095513</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>54</v>
       </c>
-      <c r="G22" s="5">
+      <c r="I22" s="5">
         <v>4.6391752577319589E-2</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>4</v>
       </c>
-      <c r="I22" s="5">
-        <f t="shared" si="1"/>
+      <c r="K22" s="5">
+        <f t="shared" si="2"/>
         <v>7.407407407407407E-2</v>
       </c>
-      <c r="J22" s="16">
+      <c r="L22" s="16">
         <v>3.4364261168384879E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3518,30 +3750,37 @@
         <v>1983</v>
       </c>
       <c r="D23">
+        <v>736</v>
+      </c>
+      <c r="E23">
         <v>7484</v>
       </c>
-      <c r="E23" s="5">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
+        <v>9.8343132014965265E-2</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="1"/>
         <v>0.26496525921966863</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>51</v>
       </c>
-      <c r="G23" s="5">
+      <c r="I23" s="5">
         <v>2.571860816944024E-2</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>14</v>
       </c>
-      <c r="I23" s="5">
-        <f t="shared" si="1"/>
+      <c r="K23" s="5">
+        <f t="shared" si="2"/>
         <v>0.27450980392156865</v>
       </c>
-      <c r="J23" s="10">
+      <c r="L23" s="10">
         <v>7.0600100857286926E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -3552,30 +3791,37 @@
         <v>2053</v>
       </c>
       <c r="D24">
+        <v>705</v>
+      </c>
+      <c r="E24">
         <v>7523</v>
       </c>
-      <c r="E24" s="5">
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
+        <v>9.3712614648411532E-2</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="1"/>
         <v>0.27289645088395587</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>52</v>
       </c>
-      <c r="G24" s="5">
+      <c r="I24" s="5">
         <v>2.532878714076961E-2</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>17</v>
       </c>
-      <c r="I24" s="5">
-        <f t="shared" si="1"/>
+      <c r="K24" s="5">
+        <f t="shared" si="2"/>
         <v>0.32692307692307693</v>
       </c>
-      <c r="J24" s="10">
+      <c r="L24" s="10">
         <v>8.2805650267900634E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -3586,30 +3832,37 @@
         <v>3800</v>
       </c>
       <c r="D25">
+        <v>8298</v>
+      </c>
+      <c r="E25">
         <v>22149</v>
       </c>
-      <c r="E25" s="5">
+      <c r="F25" s="5">
         <f t="shared" si="0"/>
+        <v>0.3746444534741975</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="1"/>
         <v>0.17156530768883471</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>53</v>
       </c>
-      <c r="G25" s="5">
+      <c r="I25" s="5">
         <v>1.394736842105263E-2</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>49</v>
       </c>
-      <c r="I25" s="8">
-        <f t="shared" si="1"/>
+      <c r="K25" s="8">
+        <f t="shared" si="2"/>
         <v>0.92452830188679247</v>
       </c>
-      <c r="J25" s="10">
+      <c r="L25" s="10">
         <v>1.2894736842105259E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -3620,139 +3873,167 @@
         <v>5268</v>
       </c>
       <c r="D26">
+        <v>7786</v>
+      </c>
+      <c r="E26">
         <v>32398</v>
       </c>
-      <c r="E26" s="5">
+      <c r="F26" s="5">
         <f t="shared" si="0"/>
+        <v>0.24032347675782456</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
         <v>0.16260262979196247</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>43</v>
       </c>
-      <c r="G26" s="5">
+      <c r="I26" s="5">
         <v>8.162490508731966E-3</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>40</v>
       </c>
-      <c r="I26" s="8">
-        <f t="shared" si="1"/>
+      <c r="K26" s="8">
+        <f t="shared" si="2"/>
         <v>0.93023255813953487</v>
       </c>
-      <c r="J26" s="10">
+      <c r="L26" s="10">
         <v>7.5930144267274107E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
         <v>761</v>
       </c>
-      <c r="E28" s="10">
-        <f>MIN(E2:E26)</f>
-        <v>0.1174878533928979</v>
+      <c r="F28" s="10">
+        <f>MIN(F2:F26)</f>
+        <v>1.6359918200408999E-2</v>
       </c>
       <c r="G28" s="10">
         <f>MIN(G2:G26)</f>
-        <v>3.2833690221270519E-3</v>
+        <v>0.1174878533928979</v>
       </c>
       <c r="I28" s="10">
         <f>MIN(I2:I26)</f>
+        <v>3.2833690221270519E-3</v>
+      </c>
+      <c r="K28" s="10">
+        <f>MIN(K2:K26)</f>
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="J28" s="10">
-        <f>MIN(J2:J26)</f>
+      <c r="L28" s="10">
+        <f>MIN(L2:L26)</f>
         <v>2.7123483226266952E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>762</v>
       </c>
-      <c r="E29" s="5">
-        <f>MAX(E2:E26)</f>
-        <v>0.55828220858895705</v>
+      <c r="F29" s="5">
+        <f>MAX(F2:F26)</f>
+        <v>0.48387517526983403</v>
       </c>
       <c r="G29" s="5">
         <f>MAX(G2:G26)</f>
-        <v>0.2893772893772894</v>
+        <v>0.55828220858895705</v>
       </c>
       <c r="I29" s="5">
         <f>MAX(I2:I26)</f>
+        <v>0.2893772893772894</v>
+      </c>
+      <c r="K29" s="5">
+        <f>MAX(K2:K26)</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="J29" s="10">
-        <f>MAX(J2:J26)</f>
+      <c r="L29" s="10">
+        <f>MAX(L2:L26)</f>
         <v>2.4111675126903549E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>763</v>
       </c>
-      <c r="E30" s="5">
-        <f>AVERAGE(E2:E26)</f>
-        <v>0.29014738619033276</v>
+      <c r="F30" s="5">
+        <f>AVERAGE(F2:F26)</f>
+        <v>0.16462284578805256</v>
       </c>
       <c r="G30" s="5">
         <f>AVERAGE(G2:G26)</f>
-        <v>3.944559100662514E-2</v>
+        <v>0.29014738619033276</v>
       </c>
       <c r="I30" s="5">
         <f>AVERAGE(I2:I26)</f>
+        <v>3.944559100662514E-2</v>
+      </c>
+      <c r="K30" s="5">
+        <f>AVERAGE(K2:K26)</f>
         <v>0.51443942419511179</v>
       </c>
-      <c r="J30" s="10">
-        <f>AVERAGE(J2:J26)</f>
+      <c r="L30" s="10">
+        <f>AVERAGE(L2:L26)</f>
         <v>1.0299703102499572E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
         <v>764</v>
       </c>
-      <c r="E31" s="5">
-        <f>MEDIAN(E2:E26)</f>
-        <v>0.27289645088395587</v>
+      <c r="F31" s="5">
+        <f>MEDIAN(F2:F26)</f>
+        <v>0.12018489984591679</v>
       </c>
       <c r="G31" s="5">
         <f>MEDIAN(G2:G26)</f>
-        <v>1.7677537336177999E-2</v>
+        <v>0.27289645088395587</v>
       </c>
       <c r="I31" s="5">
         <f>MEDIAN(I2:I26)</f>
+        <v>1.7677537336177999E-2</v>
+      </c>
+      <c r="K31" s="5">
+        <f>MEDIAN(K2:K26)</f>
         <v>0.46938775510204084</v>
       </c>
-      <c r="J31" s="10">
-        <f>MEDIAN(J2:J26)</f>
+      <c r="L31" s="10">
+        <f>MEDIAN(L2:L26)</f>
         <v>9.1269841269841275E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>765</v>
       </c>
-      <c r="E32" s="13">
-        <f>STDEVP(E2:E26)</f>
-        <v>0.10761728119565178</v>
+      <c r="F32" s="13">
+        <f>STDEVP(F2:F26)</f>
+        <v>0.12507025115671697</v>
       </c>
       <c r="G32" s="13">
         <f>STDEVP(G2:G26)</f>
-        <v>5.6778067162212481E-2</v>
+        <v>0.10761728119565178</v>
       </c>
       <c r="I32" s="13">
         <f>STDEVP(I2:I26)</f>
+        <v>5.6778067162212481E-2</v>
+      </c>
+      <c r="K32" s="13">
+        <f>STDEVP(K2:K26)</f>
         <v>0.30956572789683251</v>
       </c>
-      <c r="J32" s="13">
-        <f>STDEVP(J2:J26)</f>
+      <c r="L32" s="13">
+        <f>STDEVP(L2:L26)</f>
         <v>5.7934955369219679E-3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L26">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11735,7 +12016,7 @@
         <v>55</v>
       </c>
       <c r="E367" s="5">
-        <f t="shared" ref="E367:E372" si="0">D367/357</f>
+        <f t="shared" ref="E367:E371" si="0">D367/357</f>
         <v>0.15406162464985995</v>
       </c>
     </row>

</xml_diff>